<commit_message>
add thread async with GUI
</commit_message>
<xml_diff>
--- a/files/root.xlsx
+++ b/files/root.xlsx
@@ -55,12 +55,22 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="48"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="48"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill>
@@ -95,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,12 +397,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -401,7 +412,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update ui of GUI
</commit_message>
<xml_diff>
--- a/files/root.xlsx
+++ b/files/root.xlsx
@@ -55,12 +55,22 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="48"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="48"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill>
@@ -105,12 +115,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,12 +408,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -412,7 +423,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>